<commit_message>
add new file TRELLO.docx
</commit_message>
<xml_diff>
--- a/motacn2.xlsx
+++ b/motacn2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>MÔ TẢ CÔNG VIỆC</t>
   </si>
@@ -38,9 +38,6 @@
     <t>THỜI GIAN</t>
   </si>
   <si>
-    <t>30 phút</t>
-  </si>
-  <si>
     <t>Huỳnh Tấn Thịnh</t>
   </si>
   <si>
@@ -66,6 +63,12 @@
   </si>
   <si>
     <t>Thảo luận chức năng 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45 phút </t>
+  </si>
+  <si>
+    <t>45 phút</t>
   </si>
 </sst>
 </file>
@@ -212,65 +215,14 @@
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -290,8 +242,59 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -576,7 +579,7 @@
   <dimension ref="G11:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,109 +590,119 @@
   </cols>
   <sheetData>
     <row r="11" spans="7:13" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="3"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="16"/>
     </row>
     <row r="12" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="6" t="s">
+      <c r="I12" s="18"/>
+      <c r="J12" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="6" t="s">
+      <c r="K12" s="22"/>
+      <c r="L12" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="M12" s="8"/>
+      <c r="M12" s="25"/>
     </row>
     <row r="13" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="H13" s="9"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="14"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="27"/>
     </row>
     <row r="14" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="21" t="s">
+      <c r="I14" s="2"/>
+      <c r="J14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="22"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="24"/>
+      <c r="M14" s="7"/>
     </row>
     <row r="15" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="I15" s="16"/>
-      <c r="J15" s="21" t="s">
+      <c r="K15" s="5"/>
+      <c r="L15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K15" s="22"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="24"/>
+      <c r="M15" s="7"/>
     </row>
     <row r="16" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="H16" s="17"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="21" t="s">
+      <c r="H16" s="12"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K16" s="22"/>
-      <c r="L16" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="M16" s="24"/>
+      <c r="M16" s="7"/>
     </row>
     <row r="17" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H17" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="26"/>
-      <c r="J17" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="K17" s="22"/>
-      <c r="L17" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="M17" s="24"/>
+      <c r="H17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="9"/>
+      <c r="J17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="7"/>
     </row>
     <row r="18" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H18" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="26"/>
-      <c r="J18" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="K18" s="22"/>
-      <c r="L18" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="M18" s="24"/>
+      <c r="H18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="9"/>
+      <c r="J18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="5"/>
+      <c r="L18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:I13"/>
+    <mergeCell ref="J12:K13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:M14"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="L18:M18"/>
     <mergeCell ref="H17:I17"/>
@@ -701,12 +714,6 @@
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="L17:M17"/>
     <mergeCell ref="J16:K16"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:I13"/>
-    <mergeCell ref="J12:K13"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>